<commit_message>
updated weights & here::here stuff
</commit_message>
<xml_diff>
--- a/inst/Fast_2x24h_OGTT_study/feeding.csv.xlsx
+++ b/inst/Fast_2x24h_OGTT_study/feeding.csv.xlsx
@@ -737,8 +737,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f18153fd1d4a92a787a9d9e562be6d1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ab0e3833db82c031de4a3f0e602590a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8197e89490dc663f80df425c475dfb63">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57d494f76f6743b951aebebbdbb44cb6" ns2:_="" ns3:_="">
     <xsd:import namespace="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
     <xsd:import namespace="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
     <xsd:element name="properties">
@@ -759,6 +759,7 @@
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -829,6 +830,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a95d4ba5-ac50-4ccb-8f38-68d250b34105" elementFormDefault="qualified">
@@ -966,7 +972,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547B8A04-C292-4078-89C2-AADA124B0C9A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B959D6C-2F43-4397-B053-8E0057CC994F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>